<commit_message>
Switched around mean and median where necessary
</commit_message>
<xml_diff>
--- a/Supplemental_Tables_PB.xlsx
+++ b/Supplemental_Tables_PB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="0" windowWidth="19060" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="18280" yWindow="0" windowWidth="19060" windowHeight="20560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table S3" sheetId="3" r:id="rId1"/>
@@ -176,8 +176,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -208,7 +220,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -217,6 +229,12 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -225,6 +243,12 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -841,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1029,10 +1053,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="1">
+        <v>8.4799999999999997E-3</v>
+      </c>
+      <c r="C16" s="1">
         <v>7.1599999999999997E-3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>8.4799999999999997E-3</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>3</v>
@@ -1107,10 +1131,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="1">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="C22" s="1">
         <v>0.22320000000000001</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.27629999999999999</v>
       </c>
       <c r="D22" s="2">
         <v>2.8899999999999999E-2</v>

</xml_diff>